<commit_message>
AShot without inspirepak and jenkins propfile
</commit_message>
<xml_diff>
--- a/src/test/resources/Documents/1079/Actual/JobMaterial.xlsx
+++ b/src/test/resources/Documents/1079/Actual/JobMaterial.xlsx
@@ -80,46 +80,46 @@
     <t>Flexo press 6x0 (Varnish 1x1)</t>
   </si>
   <si>
+    <t xml:space="preserve">Black - UV - </t>
+  </si>
+  <si>
+    <t>1.05</t>
+  </si>
+  <si>
+    <t>lbs</t>
+  </si>
+  <si>
+    <t>10001817 - 9409 MIXING BLACK UV - INK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cyan - UV - </t>
+  </si>
+  <si>
+    <t>10001837 - 9443 PRO CYAN BW8 UV - INK</t>
+  </si>
+  <si>
+    <t>Varnish - UV Gloss - UV</t>
+  </si>
+  <si>
+    <t>10.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pantone-1 - UV - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellow - UV - </t>
+  </si>
+  <si>
+    <t>10001305 - PROCESS YELLOW C UV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PANTONE Yellow U  - UV - </t>
+  </si>
+  <si>
     <t xml:space="preserve">Magenta - UV - </t>
   </si>
   <si>
-    <t>1.05</t>
-  </si>
-  <si>
-    <t>lbs</t>
-  </si>
-  <si>
     <t>10001836 - 9442 PRO MAGENTA BW5 UV - INK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black - UV - </t>
-  </si>
-  <si>
-    <t>10001817 - 9409 MIXING BLACK UV - INK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cyan - UV - </t>
-  </si>
-  <si>
-    <t>10001837 - 9443 PRO CYAN BW8 UV - INK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PANTONE Yellow U  - UV - </t>
-  </si>
-  <si>
-    <t>Varnish - UV Gloss - UV</t>
-  </si>
-  <si>
-    <t>10.52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yellow - UV - </t>
-  </si>
-  <si>
-    <t>10001305 - PROCESS YELLOW C UV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pantone-1 - UV - </t>
   </si>
   <si>
     <t xml:space="preserve">Photopolymer Plate </t>
@@ -804,7 +804,7 @@
         <v>27</v>
       </c>
       <c r="E5" t="s" s="30">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s" s="31">
         <v>23</v>
@@ -813,7 +813,7 @@
         <v>16</v>
       </c>
       <c r="H5" t="s" s="33">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
@@ -856,7 +856,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="s" s="46">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s" s="47">
         <v>23</v>
@@ -865,7 +865,7 @@
         <v>16</v>
       </c>
       <c r="H7" t="s" s="49">
-        <v>16</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -891,7 +891,7 @@
         <v>16</v>
       </c>
       <c r="H8" t="s" s="57">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9">
@@ -905,7 +905,7 @@
         <v>20</v>
       </c>
       <c r="D9" t="s" s="61">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s" s="62">
         <v>22</v>
@@ -917,7 +917,7 @@
         <v>16</v>
       </c>
       <c r="H9" t="s" s="65">
-        <v>16</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">

</xml_diff>